<commit_message>
added an additional sheet
</commit_message>
<xml_diff>
--- a/IceCreamFaves.xlsx
+++ b/IceCreamFaves.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4cf2d13cb46b380c/Desktop/module 1 excel/activity 2 work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{714DE2C6-FA26-40C2-82C9-67FB98E25B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{714DE2C6-FA26-40C2-82C9-67FB98E25B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{239136C3-FAE0-4AAC-88BE-E4D631CDFE63}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1035" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="favorite flavor chart" sheetId="3" r:id="rId1"/>
-    <sheet name="flavor data" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
-    <sheet name="flavor sales" sheetId="2" r:id="rId4"/>
+    <sheet name="new sheet" sheetId="7" r:id="rId2"/>
+    <sheet name="flavor data" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
+    <sheet name="flavor sales" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'flavor sales'!$A$1:$A$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'flavor sales'!$A$1:$A$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Vanilla</t>
   </si>
@@ -136,6 +137,9 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>What in the world am I doing</t>
   </si>
 </sst>
 </file>
@@ -4382,7 +4386,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{289129C5-97D8-42F3-B211-4C82AD84D25A}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" enableDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{289129C5-97D8-42F3-B211-4C82AD84D25A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" enableDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -5072,6 +5076,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D8CF26-4EDB-4865-9AC0-F54E06FAFC73}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -5239,7 +5261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AAD9B2F-2C1D-42B3-8D99-6FB7F7566FA1}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5253,12 +5275,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3667FF1-84D2-48CC-B6F8-A437FF49202E}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>